<commit_message>
update & rectify "cartes objets personnages" system
</commit_message>
<xml_diff>
--- a/00.Memory_systems/02.Cartes/Cartes_Objet_Personnages.xlsx
+++ b/00.Memory_systems/02.Cartes/Cartes_Objet_Personnages.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097E8FAF-5EDC-4F32-9992-D1F3A7C72962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E551647E-B540-40C4-8F0F-77720C8CB64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="4560" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cartes" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="337">
   <si>
     <t>Papa</t>
   </si>
@@ -134,9 +134,6 @@
     <t>cœur (amour &amp; organe)</t>
   </si>
   <si>
-    <t>tâche, tagine - tâcher // déchet</t>
-  </si>
-  <si>
     <t>tonneau, tennis // tanné, diner</t>
   </si>
   <si>
@@ -146,15 +143,6 @@
     <t>tam-tam, tomate // damier</t>
   </si>
   <si>
-    <t>terre, tarte - (en)terrer, tarter (à la crème) // torche, tard, dard</t>
-  </si>
-  <si>
-    <t>tôle, taule - emprisonner // dalle, talon</t>
-  </si>
-  <si>
-    <t>tapis, table // taupe, tape, tabouret, tapas</t>
-  </si>
-  <si>
     <t>Objet / Action si possible</t>
   </si>
   <si>
@@ -413,18 +401,12 @@
     <t>Maman // Mat, Martin, Marc, Malik, Marianne, Marie André</t>
   </si>
   <si>
-    <t>Rom // Roxane</t>
-  </si>
-  <si>
     <t>Lolo // Lionel, Lilou</t>
   </si>
   <si>
     <t>Julien // Jeanne, Juju, Julie</t>
   </si>
   <si>
-    <t>Xav // Clem, Claude, Coco, Co</t>
-  </si>
-  <si>
     <t>Flo (cousine) //  Frank</t>
   </si>
   <si>
@@ -476,15 +458,9 @@
     <t>Freddie Mercury, // Whitney Houston, Philippe Katerine</t>
   </si>
   <si>
-    <t xml:space="preserve">Bob Marley // 2Pac, </t>
-  </si>
-  <si>
     <t>Céline Dion // Sting, Stevie, Serge Gainsbourg</t>
   </si>
   <si>
-    <t>Zitoon &amp; Sophie // Sébastien</t>
-  </si>
-  <si>
     <t>célébrité(e)s,</t>
   </si>
   <si>
@@ -1005,6 +981,60 @@
   </si>
   <si>
     <t>Co- R</t>
+  </si>
+  <si>
+    <t>terre, tour, tir // torche, tard, dard</t>
+  </si>
+  <si>
+    <t>tôle, taule, tuile // dalle, talon</t>
+  </si>
+  <si>
+    <t>tâche, toge // tagine, déchet</t>
+  </si>
+  <si>
+    <t>tapis, toupis, // table, taupe, tape, tabouret, tapas</t>
+  </si>
+  <si>
+    <t>canne, cannoé // canneton</t>
+  </si>
+  <si>
+    <t>car, karaté, carie</t>
+  </si>
+  <si>
+    <t>cale, calin // caillou</t>
+  </si>
+  <si>
+    <t>pannier, panneau // panne</t>
+  </si>
+  <si>
+    <t>pomme, piment // paume</t>
+  </si>
+  <si>
+    <t>bar, barre // part</t>
+  </si>
+  <si>
+    <t>pêle, pile // pale</t>
+  </si>
+  <si>
+    <t>pipe, papier</t>
+  </si>
+  <si>
+    <t>patate, patte à tartiner</t>
+  </si>
+  <si>
+    <t>2Pac // Bob Marley</t>
+  </si>
+  <si>
+    <t>Tom Jones // Thomas Dutronc</t>
+  </si>
+  <si>
+    <t>Rom // Roxane, Roudoudou</t>
+  </si>
+  <si>
+    <t>Carine, Xav // Clem, Claude, Coco, Co</t>
+  </si>
+  <si>
+    <t>Sophie // Sébastien, Zitoon</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CDBAAA-8D29-48BA-B8DD-36CD4CFEB934}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1405,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1394,22 +1424,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,16 +1450,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>323</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>326</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,16 +1470,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>327</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,76 +1490,76 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>319</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>324</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>81</v>
+        <v>328</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>320</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>54</v>
+        <v>325</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>329</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>321</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B10" s="2">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1540,16 +1570,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,36 +1590,36 @@
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>322</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>330</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1600,53 +1630,53 @@
         <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>331</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>35</v>
@@ -1659,19 +1689,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1690,25 +1720,25 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1722,16 +1752,16 @@
         <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1742,19 +1772,19 @@
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1765,91 +1795,91 @@
         <v>4</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>129</v>
+        <v>334</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B27" s="2">
         <v>6</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B28" s="2">
         <v>7</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>132</v>
+        <v>335</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1860,19 +1890,19 @@
         <v>8</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1883,42 +1913,42 @@
         <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>150</v>
+        <v>332</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I30" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2">
         <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>152</v>
+        <v>336</v>
       </c>
       <c r="I31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1929,59 +1959,59 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>144</v>
+        <v>333</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I34" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1989,12 +2019,12 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D37" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D38" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +2038,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,79 +2050,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -2100,71 +2130,71 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -2172,15 +2202,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -2188,31 +2218,31 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -2220,167 +2250,167 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -2388,47 +2418,47 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B48" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B52" t="s">
         <v>35</v>
@@ -2459,7 +2489,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2469,15 +2499,15 @@
         <v>Tr -  A</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -2487,15 +2517,15 @@
         <v>Tr -  2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -2505,15 +2535,15 @@
         <v>Tr -  3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -2523,15 +2553,15 @@
         <v>Tr -  4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2541,15 +2571,15 @@
         <v>Tr -  5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
@@ -2559,15 +2589,15 @@
         <v>Tr -  6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
@@ -2577,15 +2607,15 @@
         <v>Tr -  7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2">
         <v>8</v>
@@ -2595,15 +2625,15 @@
         <v>Tr -  8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
@@ -2613,15 +2643,15 @@
         <v>Tr -  9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
@@ -2631,7 +2661,7 @@
         <v>Tr -  10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -2639,7 +2669,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
@@ -2649,15 +2679,15 @@
         <v>Tr -  V</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -2667,15 +2697,15 @@
         <v>Tr -  D</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
@@ -2685,15 +2715,15 @@
         <v>Tr -  R</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -2703,15 +2733,15 @@
         <v>Ca -  A</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -2721,15 +2751,15 @@
         <v>Ca -  2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -2739,15 +2769,15 @@
         <v>Ca -  3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
@@ -2757,15 +2787,15 @@
         <v>Ca -  4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
@@ -2775,15 +2805,15 @@
         <v>Ca -  5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B19" s="2">
         <v>6</v>
@@ -2793,7 +2823,7 @@
         <v>Ca -  6</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -2801,7 +2831,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B20" s="2">
         <v>7</v>
@@ -2811,15 +2841,15 @@
         <v>Ca -  7</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F20" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2">
         <v>8</v>
@@ -2829,7 +2859,7 @@
         <v>Ca -  8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -2837,7 +2867,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2">
         <v>9</v>
@@ -2847,15 +2877,15 @@
         <v>Ca -  9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B23" s="2">
         <v>10</v>
@@ -2865,15 +2895,15 @@
         <v>Ca -  10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F23" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>27</v>
@@ -2883,15 +2913,15 @@
         <v>Ca -  V</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
@@ -2901,7 +2931,7 @@
         <v>Ca -  D</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F25" t="s">
         <v>25</v>
@@ -2909,7 +2939,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>29</v>
@@ -2919,15 +2949,15 @@
         <v>Ca -  R</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
@@ -2937,15 +2967,15 @@
         <v>Pi -  A</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2">
         <v>2</v>
@@ -2955,15 +2985,15 @@
         <v>Pi -  2</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
@@ -2973,15 +3003,15 @@
         <v>Pi -  3</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B30" s="2">
         <v>4</v>
@@ -2991,15 +3021,15 @@
         <v>Pi -  4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2">
         <v>5</v>
@@ -3009,15 +3039,15 @@
         <v>Pi -  5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B32" s="2">
         <v>6</v>
@@ -3027,15 +3057,15 @@
         <v>Pi -  6</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B33" s="2">
         <v>7</v>
@@ -3045,15 +3075,15 @@
         <v>Pi -  7</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B34" s="2">
         <v>8</v>
@@ -3063,15 +3093,15 @@
         <v>Pi -  8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F34" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B35" s="2">
         <v>9</v>
@@ -3081,15 +3111,15 @@
         <v>Pi -  9</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B36" s="2">
         <v>10</v>
@@ -3099,15 +3129,15 @@
         <v>Pi -  10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>27</v>
@@ -3117,15 +3147,15 @@
         <v>Pi -  V</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>28</v>
@@ -3135,15 +3165,15 @@
         <v>Pi -  D</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>29</v>
@@ -3153,15 +3183,15 @@
         <v>Pi -  R</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>26</v>
@@ -3171,15 +3201,15 @@
         <v>Co -  A</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B41" s="2">
         <v>2</v>
@@ -3189,15 +3219,15 @@
         <v>Co -  2</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F41" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B42" s="2">
         <v>3</v>
@@ -3207,15 +3237,15 @@
         <v>Co -  3</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="F42" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B43" s="2">
         <v>4</v>
@@ -3225,15 +3255,15 @@
         <v>Co -  4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F43" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B44" s="2">
         <v>5</v>
@@ -3243,15 +3273,15 @@
         <v>Co -  5</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F44" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B45" s="2">
         <v>6</v>
@@ -3261,15 +3291,15 @@
         <v>Co -  6</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B46" s="2">
         <v>7</v>
@@ -3279,7 +3309,7 @@
         <v>Co -  7</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -3287,7 +3317,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B47" s="2">
         <v>8</v>
@@ -3297,15 +3327,15 @@
         <v>Co -  8</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F47" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B48" s="2">
         <v>9</v>
@@ -3315,15 +3345,15 @@
         <v>Co -  9</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2">
         <v>10</v>
@@ -3333,15 +3363,15 @@
         <v>Co -  10</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F49" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>27</v>
@@ -3351,15 +3381,15 @@
         <v>Co -  V</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F50" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>28</v>
@@ -3369,15 +3399,15 @@
         <v>Co -  D</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F51" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>29</v>
@@ -3387,7 +3417,7 @@
         <v>Co -  R</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F52" t="s">
         <v>35</v>
@@ -3420,45 +3450,45 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="7" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="7" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="F3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="7" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -3468,7 +3498,7 @@
         <v>Tr -  A</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -3476,7 +3506,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
@@ -3486,7 +3516,7 @@
         <v>Tr -  2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
@@ -3495,7 +3525,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -3505,16 +3535,16 @@
         <v>Tr -  3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -3524,16 +3554,16 @@
         <v>Tr -  4</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -3543,16 +3573,16 @@
         <v>Tr -  5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
@@ -3562,16 +3592,16 @@
         <v>Tr -  6</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
@@ -3581,16 +3611,16 @@
         <v>Tr -  7</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
@@ -3600,7 +3630,7 @@
         <v>Tr -  8</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F12" t="s">
         <v>23</v>
@@ -3608,7 +3638,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
@@ -3618,15 +3648,15 @@
         <v>Tr -  9</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
@@ -3636,15 +3666,15 @@
         <v>Tr -  10</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F14" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
@@ -3654,15 +3684,15 @@
         <v>Tr -  V</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F15" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>28</v>
@@ -3672,15 +3702,15 @@
         <v>Tr -  D</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>29</v>
@@ -3690,15 +3720,15 @@
         <v>Tr -  R</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F17" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>26</v>
@@ -3708,7 +3738,7 @@
         <v>Ca -  A</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -3716,7 +3746,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
@@ -3726,15 +3756,15 @@
         <v>Ca -  2</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
@@ -3744,15 +3774,15 @@
         <v>Ca -  3</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F20" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2">
         <v>4</v>
@@ -3762,15 +3792,15 @@
         <v>Ca -  4</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2">
         <v>5</v>
@@ -3780,15 +3810,15 @@
         <v>Ca -  5</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B23" s="2">
         <v>6</v>
@@ -3798,7 +3828,7 @@
         <v>Ca -  6</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -3806,7 +3836,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B24" s="2">
         <v>7</v>
@@ -3816,15 +3846,15 @@
         <v>Ca -  7</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B25" s="2">
         <v>8</v>
@@ -3834,15 +3864,15 @@
         <v>Ca -  8</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F25" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B26" s="2">
         <v>9</v>
@@ -3852,7 +3882,7 @@
         <v>Ca -  9</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -3860,7 +3890,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B27" s="2">
         <v>10</v>
@@ -3870,7 +3900,7 @@
         <v>Ca -  10</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -3878,7 +3908,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
@@ -3888,15 +3918,15 @@
         <v>Ca -  V</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F28" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
@@ -3906,15 +3936,15 @@
         <v>Ca -  D</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>29</v>
@@ -3924,7 +3954,7 @@
         <v>Ca -  R</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
@@ -3932,7 +3962,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
@@ -3942,7 +3972,7 @@
         <v>Pi -  A</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -3950,7 +3980,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B32" s="2">
         <v>2</v>
@@ -3960,7 +3990,7 @@
         <v>Pi -  2</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F32" t="s">
         <v>24</v>
@@ -3968,7 +3998,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B33" s="2">
         <v>3</v>
@@ -3978,15 +4008,15 @@
         <v>Pi -  3</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F33" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B34" s="2">
         <v>4</v>
@@ -3996,15 +4026,15 @@
         <v>Pi -  4</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F34" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B35" s="2">
         <v>5</v>
@@ -4014,15 +4044,15 @@
         <v>Pi -  5</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F35" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B36" s="2">
         <v>6</v>
@@ -4032,15 +4062,15 @@
         <v>Pi -  6</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F36" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B37" s="2">
         <v>7</v>
@@ -4050,15 +4080,15 @@
         <v>Pi -  7</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B38" s="2">
         <v>8</v>
@@ -4068,15 +4098,15 @@
         <v>Pi -  8</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F38" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B39" s="2">
         <v>9</v>
@@ -4086,15 +4116,15 @@
         <v>Pi -  9</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F39" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B40" s="2">
         <v>10</v>
@@ -4104,15 +4134,15 @@
         <v>Pi -  10</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F40" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>27</v>
@@ -4122,15 +4152,15 @@
         <v>Pi -  V</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>28</v>
@@ -4140,15 +4170,15 @@
         <v>Pi -  D</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F42" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>29</v>
@@ -4158,15 +4188,15 @@
         <v>Pi -  R</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F43" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>26</v>
@@ -4176,7 +4206,7 @@
         <v>Co -  A</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
@@ -4184,7 +4214,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B45" s="2">
         <v>2</v>
@@ -4194,7 +4224,7 @@
         <v>Co -  2</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F45" t="s">
         <v>2</v>
@@ -4202,7 +4232,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B46" s="2">
         <v>3</v>
@@ -4212,7 +4242,7 @@
         <v>Co -  3</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -4220,7 +4250,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B47" s="2">
         <v>4</v>
@@ -4230,7 +4260,7 @@
         <v>Co -  4</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F47" t="s">
         <v>4</v>
@@ -4238,7 +4268,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B48" s="2">
         <v>5</v>
@@ -4248,15 +4278,15 @@
         <v>Co -  5</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F48" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2">
         <v>6</v>
@@ -4266,15 +4296,15 @@
         <v>Co -  6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F49" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B50" s="2">
         <v>7</v>
@@ -4284,15 +4314,15 @@
         <v>Co -  7</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F50" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B51" s="2">
         <v>8</v>
@@ -4302,15 +4332,15 @@
         <v>Co -  8</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F51" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B52" s="2">
         <v>9</v>
@@ -4320,7 +4350,7 @@
         <v>Co -  9</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F52" t="s">
         <v>0</v>
@@ -4328,7 +4358,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B53" s="2">
         <v>10</v>
@@ -4338,15 +4368,15 @@
         <v>Co -  10</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F53" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>27</v>
@@ -4356,15 +4386,15 @@
         <v>Co -  V</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F54" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>28</v>
@@ -4374,15 +4404,15 @@
         <v>Co -  D</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>29</v>
@@ -4392,10 +4422,10 @@
         <v>Co -  R</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F56" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4408,7 +4438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1928CB2D-D63E-48EC-8B03-6743D57F98E9}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C22" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
@@ -4421,39 +4451,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4461,7 +4491,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -4470,52 +4500,52 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -4523,47 +4553,47 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -4571,39 +4601,39 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -4611,23 +4641,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B24" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -4635,7 +4665,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4643,23 +4673,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B29" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -4667,7 +4697,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -4675,7 +4705,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -4683,95 +4713,95 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B33" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B34" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B39" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B40" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -4779,7 +4809,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
@@ -4787,7 +4817,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
@@ -4795,7 +4825,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
@@ -4803,39 +4833,39 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B48" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B50" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
@@ -4843,34 +4873,34 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>